<commit_message>
Updated all file.py and Added a file.xlxs
</commit_message>
<xml_diff>
--- a/BTScrapDaTa03/Musicians.xlsx
+++ b/BTScrapDaTa03/Musicians.xlsx
@@ -27,84 +27,164 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="80">
   <si>
     <t>Name</t>
   </si>
   <si>
+    <t>Year active</t>
+  </si>
+  <si>
     <t>The 13th Floor Elevators</t>
   </si>
   <si>
+    <t>1965–1969, 1973, 1984, 2015</t>
+  </si>
+  <si>
     <t>Alice Cooper (band)</t>
   </si>
   <si>
+    <t>1968–1974
+(reunions: 1999, 2006, 2010, 2011, 2015, 2017, 2019)</t>
+  </si>
+  <si>
     <t>The Amboy Dukes (band)</t>
   </si>
   <si>
+    <t>1964–1975</t>
+  </si>
+  <si>
     <t>Amon Düül</t>
   </si>
   <si>
+    <t>1967–1971, 1980–1989</t>
+  </si>
+  <si>
     <t>Big Brother and the Holding Company</t>
   </si>
   <si>
+    <t>1965–1968, 1969–1972, 1987–present</t>
+  </si>
+  <si>
     <t>Black Sabbath</t>
   </si>
   <si>
+    <t>1968–2017 (hiatuses: 1984–1985, 1996–1997, 2006–2011)</t>
+  </si>
+  <si>
     <t>Blue Cheer</t>
   </si>
   <si>
+    <t>1966–2009</t>
+  </si>
+  <si>
     <t>Blues Magoos</t>
   </si>
   <si>
+    <t>1964–1970, 2008–present</t>
+  </si>
+  <si>
     <t>The Charlatans (American band)</t>
   </si>
   <si>
+    <t>1964–1969 1997 2005 2015</t>
+  </si>
+  <si>
     <t>Count Five</t>
   </si>
   <si>
+    <t>1964–1969</t>
+  </si>
+  <si>
     <t>Country Joe and the Fish</t>
   </si>
   <si>
+    <t>1965–1970, 1977, 2004–2006 (as Country Joe Band), sporadically thereafter</t>
+  </si>
+  <si>
     <t>Coven (band)</t>
   </si>
   <si>
+    <t>1967–1975, 2007–present</t>
+  </si>
+  <si>
     <t>Cream (band)</t>
   </si>
   <si>
+    <t>1966–1968 1993 2005</t>
+  </si>
+  <si>
     <t>Deep Purple</t>
   </si>
   <si>
+    <t>1968–19761984–present</t>
+  </si>
+  <si>
     <t>The Deviants (band)</t>
   </si>
   <si>
+    <t>1966–196919781984199620022011–2013</t>
+  </si>
+  <si>
     <t>The Doors</t>
   </si>
   <si>
+    <t>1965–19731978
+One-off reunions: 1993, 1997, 2000, 2011–2012, 2012–2013</t>
+  </si>
+  <si>
     <t>The Electric Prunes</t>
   </si>
   <si>
+    <t>1965–1970, 1999–present</t>
+  </si>
+  <si>
     <t>The Fugs</t>
   </si>
   <si>
+    <t>1964–1969 1984–present</t>
+  </si>
+  <si>
     <t>Grateful Dead</t>
   </si>
   <si>
+    <t>1965–1995</t>
+  </si>
+  <si>
     <t>The Great Society (band)</t>
   </si>
   <si>
+    <t>1965–1966</t>
+  </si>
+  <si>
     <t>The Groundhogs</t>
   </si>
   <si>
+    <t>1963–2014</t>
+  </si>
+  <si>
     <t>Hawkwind</t>
   </si>
   <si>
+    <t>1969–present</t>
+  </si>
+  <si>
     <t>Iron Butterfly</t>
   </si>
   <si>
+    <t>1966–19711974–19851987–20122015–2021</t>
+  </si>
+  <si>
     <t>Jefferson Airplane</t>
   </si>
   <si>
-    <t>The Jimi Hendrix Experience</t>
+    <t>1965–1973, 1989, 1996</t>
+  </si>
+  <si>
+    <t>Jimi Hendrix</t>
+  </si>
+  <si>
+    <t>1962–1970</t>
   </si>
   <si>
     <t>Janis Joplin</t>
@@ -113,166 +193,84 @@
     <t>JPT Scare Band</t>
   </si>
   <si>
+    <t>1973–present</t>
+  </si>
+  <si>
     <t>Love (band)</t>
   </si>
   <si>
+    <t>1965–1996 2002–2005 2009–present</t>
+  </si>
+  <si>
     <t>MC5</t>
   </si>
   <si>
+    <t>1963–19721974–197519922003–20112018–20192022–2024</t>
+  </si>
+  <si>
     <t>Moby Grape</t>
   </si>
   <si>
+    <t>1966–196919711973–19751977–19791983–19841987–19911996–20012006–present</t>
+  </si>
+  <si>
     <t>The Music Machine</t>
   </si>
   <si>
+    <t>1965–1969</t>
+  </si>
+  <si>
     <t>Pop Mašina</t>
   </si>
   <si>
+    <t>1972–1978</t>
+  </si>
+  <si>
     <t>Quicksilver Messenger Service</t>
   </si>
   <si>
+    <t>1965–1979, 2006–2009
+1984–1996 (Gary Duncan's Quicksilver)
+2009–present (David Freiberg's Quicksilver Messenger Service)</t>
+  </si>
+  <si>
     <t>Santana (band)</t>
   </si>
   <si>
+    <t>1966–present</t>
+  </si>
+  <si>
     <t>The Seeds</t>
   </si>
   <si>
+    <t>1965–1969, 1969–1972 (as Sky Saxon and the Seeds), 1989, 2003–2009, 2017–present (as Daryl Hooper and the Seeds)</t>
+  </si>
+  <si>
     <t>Grace Slick</t>
   </si>
   <si>
     <t>Steppenwolf (band)</t>
   </si>
   <si>
+    <t>1967–19721974–19761980–2018</t>
+  </si>
+  <si>
     <t>Tully (band)</t>
   </si>
   <si>
+    <t>1968–1972, 1976–1978</t>
+  </si>
+  <si>
     <t>Vanilla Fudge</t>
   </si>
   <si>
+    <t>1967–19701982–19841987–198819911999–present</t>
+  </si>
+  <si>
     <t>Wooden Shjips</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
-    <t>https://en.wikipedia.org/wiki/The_13th_Floor_Elevators</t>
-  </si>
-  <si>
-    <t>https://en.wikipedia.org/wiki/Alice_Cooper_(band)</t>
-  </si>
-  <si>
-    <t>https://en.wikipedia.org/wiki/The_Amboy_Dukes_(band)</t>
-  </si>
-  <si>
-    <t>https://en.wikipedia.org/wiki/Amon_D%C3%BC%C3%BCl</t>
-  </si>
-  <si>
-    <t>https://en.wikipedia.org/wiki/Big_Brother_and_the_Holding_Company</t>
-  </si>
-  <si>
-    <t>https://en.wikipedia.org/wiki/Black_Sabbath</t>
-  </si>
-  <si>
-    <t>https://en.wikipedia.org/wiki/Blue_Cheer</t>
-  </si>
-  <si>
-    <t>https://en.wikipedia.org/wiki/Blues_Magoos</t>
-  </si>
-  <si>
-    <t>https://en.wikipedia.org/wiki/The_Charlatans_(American_band)</t>
-  </si>
-  <si>
-    <t>https://en.wikipedia.org/wiki/Count_Five</t>
-  </si>
-  <si>
-    <t>https://en.wikipedia.org/wiki/Country_Joe_and_the_Fish</t>
-  </si>
-  <si>
-    <t>https://en.wikipedia.org/wiki/Coven_(band)</t>
-  </si>
-  <si>
-    <t>https://en.wikipedia.org/wiki/Cream_(band)</t>
-  </si>
-  <si>
-    <t>https://en.wikipedia.org/wiki/Deep_Purple</t>
-  </si>
-  <si>
-    <t>https://en.wikipedia.org/wiki/The_Deviants_(band)</t>
-  </si>
-  <si>
-    <t>https://en.wikipedia.org/wiki/The_Doors</t>
-  </si>
-  <si>
-    <t>https://en.wikipedia.org/wiki/The_Electric_Prunes</t>
-  </si>
-  <si>
-    <t>https://en.wikipedia.org/wiki/The_Fugs</t>
-  </si>
-  <si>
-    <t>https://en.wikipedia.org/wiki/Grateful_Dead</t>
-  </si>
-  <si>
-    <t>https://en.wikipedia.org/wiki/The_Great_Society_(band)</t>
-  </si>
-  <si>
-    <t>https://en.wikipedia.org/wiki/The_Groundhogs</t>
-  </si>
-  <si>
-    <t>https://en.wikipedia.org/wiki/Hawkwind</t>
-  </si>
-  <si>
-    <t>https://en.wikipedia.org/wiki/Iron_Butterfly</t>
-  </si>
-  <si>
-    <t>https://en.wikipedia.org/wiki/Jefferson_Airplane</t>
-  </si>
-  <si>
-    <t>https://en.wikipedia.org/wiki/The_Jimi_Hendrix_Experience</t>
-  </si>
-  <si>
-    <t>https://en.wikipedia.org/wiki/Janis_Joplin</t>
-  </si>
-  <si>
-    <t>https://en.wikipedia.org/wiki/JPT_Scare_Band</t>
-  </si>
-  <si>
-    <t>https://en.wikipedia.org/wiki/Love_(band)</t>
-  </si>
-  <si>
-    <t>https://en.wikipedia.org/wiki/MC5</t>
-  </si>
-  <si>
-    <t>https://en.wikipedia.org/wiki/Moby_Grape</t>
-  </si>
-  <si>
-    <t>https://en.wikipedia.org/wiki/The_Music_Machine</t>
-  </si>
-  <si>
-    <t>https://en.wikipedia.org/wiki/Pop_Ma%C5%A1ina</t>
-  </si>
-  <si>
-    <t>https://en.wikipedia.org/wiki/Quicksilver_Messenger_Service</t>
-  </si>
-  <si>
-    <t>https://en.wikipedia.org/wiki/Santana_(band)</t>
-  </si>
-  <si>
-    <t>https://en.wikipedia.org/wiki/The_Seeds</t>
-  </si>
-  <si>
-    <t>https://en.wikipedia.org/wiki/Grace_Slick</t>
-  </si>
-  <si>
-    <t>https://en.wikipedia.org/wiki/Steppenwolf_(band)</t>
-  </si>
-  <si>
-    <t>https://en.wikipedia.org/wiki/Tully_(band)</t>
-  </si>
-  <si>
-    <t>https://en.wikipedia.org/wiki/Vanilla_Fudge</t>
-  </si>
-  <si>
-    <t>https://en.wikipedia.org/wiki/Wooden_Shjips</t>
+    <t>2006–present</t>
   </si>
 </sst>
 </file>
@@ -301,18 +299,18 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -770,28 +768,28 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -915,12 +913,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1267,276 +1264,467 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AP2"/>
+  <dimension ref="A1:C41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B43" sqref="B43:B44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="2"/>
   <cols>
-    <col min="2" max="2" width="22.7777777777778" customWidth="1"/>
-    <col min="3" max="3" width="48.7777777777778" customWidth="1"/>
-    <col min="4" max="4" width="35.3333333333333" customWidth="1"/>
+    <col min="2" max="2" width="38.7777777777778" customWidth="1"/>
+    <col min="3" max="3" width="104.333333333333" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:42">
+    <row r="1" spans="2:3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AK1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="AL1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AM1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="AN1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AO1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AP1" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:42">
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="2" t="s">
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="1">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
         <v>42</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C22" t="s">
         <v>43</v>
       </c>
-      <c r="E2" t="s">
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="1">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
         <v>44</v>
       </c>
-      <c r="F2" t="s">
+      <c r="C23" t="s">
         <v>45</v>
       </c>
-      <c r="G2" t="s">
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="1">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
         <v>46</v>
       </c>
-      <c r="H2" t="s">
+      <c r="C24" t="s">
         <v>47</v>
       </c>
-      <c r="I2" t="s">
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="1">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
         <v>48</v>
       </c>
-      <c r="J2" t="s">
+      <c r="C25" t="s">
         <v>49</v>
       </c>
-      <c r="K2" t="s">
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="1">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
         <v>50</v>
       </c>
-      <c r="L2" t="s">
+      <c r="C26" t="s">
         <v>51</v>
       </c>
-      <c r="M2" t="s">
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="1">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
         <v>52</v>
       </c>
-      <c r="N2" t="s">
+      <c r="C27" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="1">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
         <v>53</v>
       </c>
-      <c r="O2" t="s">
+      <c r="C28" t="s">
         <v>54</v>
       </c>
-      <c r="P2" t="s">
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="1">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
         <v>55</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="C29" t="s">
         <v>56</v>
       </c>
-      <c r="R2" t="s">
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="1">
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
         <v>57</v>
       </c>
-      <c r="S2" t="s">
+      <c r="C30" t="s">
         <v>58</v>
       </c>
-      <c r="T2" t="s">
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="1">
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
         <v>59</v>
       </c>
-      <c r="U2" t="s">
+      <c r="C31" t="s">
         <v>60</v>
       </c>
-      <c r="V2" t="s">
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="1">
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
         <v>61</v>
       </c>
-      <c r="W2" t="s">
+      <c r="C32" t="s">
         <v>62</v>
       </c>
-      <c r="X2" t="s">
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="1">
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
         <v>63</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="C33" t="s">
         <v>64</v>
       </c>
-      <c r="Z2" t="s">
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="1">
+        <v>32</v>
+      </c>
+      <c r="B34" t="s">
         <v>65</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="C34" t="s">
         <v>66</v>
       </c>
-      <c r="AB2" t="s">
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="1">
+        <v>33</v>
+      </c>
+      <c r="B35" t="s">
         <v>67</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="C35" t="s">
         <v>68</v>
       </c>
-      <c r="AD2" t="s">
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="1">
+        <v>34</v>
+      </c>
+      <c r="B36" t="s">
         <v>69</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="C36" t="s">
         <v>70</v>
       </c>
-      <c r="AF2" t="s">
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="1">
+        <v>35</v>
+      </c>
+      <c r="B37" t="s">
         <v>71</v>
       </c>
-      <c r="AG2" t="s">
+      <c r="C37" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="1">
+        <v>36</v>
+      </c>
+      <c r="B38" t="s">
         <v>72</v>
       </c>
-      <c r="AH2" t="s">
+      <c r="C38" t="s">
         <v>73</v>
       </c>
-      <c r="AI2" t="s">
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="1">
+        <v>37</v>
+      </c>
+      <c r="B39" t="s">
         <v>74</v>
       </c>
-      <c r="AJ2" t="s">
+      <c r="C39" t="s">
         <v>75</v>
       </c>
-      <c r="AK2" t="s">
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="1">
+        <v>38</v>
+      </c>
+      <c r="B40" t="s">
         <v>76</v>
       </c>
-      <c r="AL2" t="s">
+      <c r="C40" t="s">
         <v>77</v>
       </c>
-      <c r="AM2" t="s">
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="1">
+        <v>39</v>
+      </c>
+      <c r="B41" t="s">
         <v>78</v>
       </c>
-      <c r="AN2" t="s">
+      <c r="C41" t="s">
         <v>79</v>
       </c>
-      <c r="AO2" t="s">
-        <v>80</v>
-      </c>
-      <c r="AP2" t="s">
-        <v>81</v>
-      </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="https://en.wikipedia.org/wiki/The_13th_Floor_Elevators"/>
-  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>

</xml_diff>